<commit_message>
Modify algorithm for scoring process, namely, score based on percentile distribution and normalized beta. Need to improve error handling as alternative method of using calculated fund params using t-bills and s&p are disabled.
</commit_message>
<xml_diff>
--- a/nicnbk-data/nicnbk-data-service-impl/src/main/resources/export_template/hf_scoring/HF_SCORING_QUALIFIED_TEMPLATE.xlsx
+++ b/nicnbk-data/nicnbk-data-service-impl/src/main/resources/export_template/hf_scoring/HF_SCORING_QUALIFIED_TEMPLATE.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\magzumov\IdeaProjects\unic\nicnbk-data\nicnbk-data-service-impl\src\main\resources\export_template\hf_scoring\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tleugabylov\IdeaProjects\projects\nicnbk-data\nicnbk-data-service-impl\src\main\resources\export_template\hf_scoring\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D19DC19-47CF-4668-81A6-6CBA535349A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24810" windowHeight="5085"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -95,10 +96,9 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
-    <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -273,7 +273,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -286,32 +286,14 @@
     <xf numFmtId="4" fontId="2" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="3" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="10" fontId="2" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="4" fontId="2" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="164" fontId="2" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="164" fontId="2" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="10" fontId="2" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -333,9 +315,21 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -617,11 +611,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -636,78 +630,78 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="15"/>
-      <c r="B2" s="16" t="s">
+      <c r="A2" s="9"/>
+      <c r="B2" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="C2" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="17"/>
+      <c r="E2" s="11"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="15"/>
-      <c r="B3" s="16" t="s">
+      <c r="A3" s="9"/>
+      <c r="B3" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="17"/>
+      <c r="E3" s="11"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="15"/>
-      <c r="B4" s="16" t="s">
+      <c r="A4" s="9"/>
+      <c r="B4" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="17"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="17"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="11"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="15"/>
-      <c r="B5" s="16" t="s">
+      <c r="A5" s="9"/>
+      <c r="B5" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="17"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="17"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="11"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="15"/>
-      <c r="B6" s="16" t="s">
+      <c r="A6" s="9"/>
+      <c r="B6" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="17"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="17"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="11"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="15"/>
-      <c r="B7" s="16" t="s">
+      <c r="A7" s="9"/>
+      <c r="B7" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="17"/>
-      <c r="E7" s="17"/>
+      <c r="C7" s="11"/>
+      <c r="E7" s="11"/>
     </row>
     <row r="8" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="18" t="s">
+      <c r="A8" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="18" t="s">
+      <c r="B8" s="12" t="s">
         <v>1</v>
       </c>
       <c r="C8" s="1" t="s">
@@ -722,17 +716,17 @@
       <c r="F8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G8" s="18" t="s">
+      <c r="G8" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="H8" s="18"/>
-      <c r="I8" s="19" t="s">
+      <c r="H8" s="12"/>
+      <c r="I8" s="13" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="18"/>
-      <c r="B9" s="18"/>
+      <c r="A9" s="12"/>
+      <c r="B9" s="12"/>
       <c r="C9" s="3" t="s">
         <v>8</v>
       </c>
@@ -751,27 +745,27 @@
       <c r="H9" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="I9" s="20"/>
+      <c r="I9" s="14"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="8"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
-      <c r="B11" s="14"/>
-      <c r="C11" s="13"/>
+      <c r="B11" s="18"/>
+      <c r="C11" s="20"/>
       <c r="D11" s="5"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="11"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="20"/>
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
     </row>

</xml_diff>